<commit_message>
Working Monthly output with new parent of children. Need to add values column data selection (date, description, price). Need to also update so that current value is exported into tree instead of min value. We dont need a min and max value we only need a Current and max value.
</commit_message>
<xml_diff>
--- a/MonthlyExpenses.xlsx
+++ b/MonthlyExpenses.xlsx
@@ -455,12 +455,12 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>90</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>150</t>
         </is>
       </c>
     </row>
@@ -472,12 +472,12 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -489,12 +489,12 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -525,12 +525,12 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>90</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>150</t>
         </is>
       </c>
     </row>
@@ -542,12 +542,12 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -559,12 +559,12 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -595,12 +595,12 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>90</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>150</t>
         </is>
       </c>
     </row>
@@ -612,12 +612,12 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -629,12 +629,12 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -665,12 +665,12 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>90</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>150</t>
         </is>
       </c>
     </row>
@@ -682,12 +682,12 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -699,12 +699,12 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -735,12 +735,12 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>90</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>150</t>
         </is>
       </c>
     </row>
@@ -752,12 +752,12 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -769,12 +769,12 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -805,12 +805,12 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>90</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>150</t>
         </is>
       </c>
     </row>
@@ -822,12 +822,12 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -839,12 +839,12 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -875,12 +875,12 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>90</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>150</t>
         </is>
       </c>
     </row>
@@ -892,12 +892,12 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -909,12 +909,12 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -945,12 +945,12 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>90</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>150</t>
         </is>
       </c>
     </row>
@@ -962,12 +962,12 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -979,12 +979,12 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1015,12 +1015,12 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>90</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>150</t>
         </is>
       </c>
     </row>
@@ -1032,12 +1032,12 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1049,12 +1049,12 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1085,12 +1085,12 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>90</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>150</t>
         </is>
       </c>
     </row>
@@ -1102,12 +1102,12 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1119,12 +1119,12 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1155,12 +1155,12 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>90</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>150</t>
         </is>
       </c>
     </row>
@@ -1172,12 +1172,12 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1189,12 +1189,12 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1225,12 +1225,12 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>90</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>150</t>
         </is>
       </c>
     </row>
@@ -1242,12 +1242,12 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1259,12 +1259,12 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Resolved monthly association issue but now I have to solve issue with averaging zero values and creditting vs debitting.
</commit_message>
<xml_diff>
--- a/MonthlyExpenses.xlsx
+++ b/MonthlyExpenses.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,24 +450,24 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Botox</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -493,6 +493,23 @@
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>God</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -509,7 +526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,24 +537,24 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Botox</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -563,6 +580,23 @@
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>God</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -579,7 +613,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,24 +624,24 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Botox</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -633,6 +667,23 @@
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>God</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -649,7 +700,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -660,24 +711,24 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Botox</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -703,6 +754,23 @@
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>God</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -719,7 +787,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -730,24 +798,24 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Botox</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -773,6 +841,23 @@
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>God</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -789,7 +874,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -800,24 +885,24 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Botox</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -843,6 +928,23 @@
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>God</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -859,7 +961,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -870,24 +972,24 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Botox</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -913,6 +1015,23 @@
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>God</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -929,7 +1048,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -940,24 +1059,24 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Botox</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -983,6 +1102,23 @@
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>God</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -999,7 +1135,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1010,24 +1146,24 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Botox</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -1053,6 +1189,23 @@
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>God</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1069,7 +1222,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1080,24 +1233,24 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Botox</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -1123,6 +1276,23 @@
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>God</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1139,7 +1309,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1150,24 +1320,24 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Botox</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -1193,6 +1363,23 @@
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>God</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1209,7 +1396,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1220,24 +1407,24 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Botox</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>90</t>
+          <t>0</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Rent</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -1263,6 +1450,23 @@
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>God</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>

<commit_message>
Resolved issue with values not being output into spreadsheet. Also rounded values off to 2 decimal places.
</commit_message>
<xml_diff>
--- a/MonthlyExpenses.xlsx
+++ b/MonthlyExpenses.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,7 +450,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Botox</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -467,7 +467,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Income</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -501,7 +501,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>God</t>
+          <t>Investments</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -510,6 +510,125 @@
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Rent</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Transitionary</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Giving</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>LLC</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Kota</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Necessities</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -526,7 +645,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,7 +656,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Botox</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -554,7 +673,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Income</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -588,7 +707,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>God</t>
+          <t>Investments</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -597,6 +716,125 @@
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Rent</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Transitionary</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Giving</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>LLC</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Kota</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Necessities</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -613,7 +851,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -624,7 +862,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Botox</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -641,7 +879,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Income</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -675,7 +913,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>God</t>
+          <t>Investments</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -684,6 +922,125 @@
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Rent</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Transitionary</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Giving</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>LLC</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Kota</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Necessities</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -700,7 +1057,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -711,7 +1068,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Botox</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -728,7 +1085,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Income</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -762,7 +1119,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>God</t>
+          <t>Investments</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -771,6 +1128,125 @@
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Rent</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Transitionary</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Giving</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>LLC</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Kota</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Necessities</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -787,7 +1263,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -798,7 +1274,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Botox</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -815,7 +1291,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Income</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -849,7 +1325,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>God</t>
+          <t>Investments</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -858,6 +1334,125 @@
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Rent</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Transitionary</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Giving</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>LLC</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Kota</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Necessities</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -874,7 +1469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -885,7 +1480,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Botox</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -902,7 +1497,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Income</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -936,7 +1531,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>God</t>
+          <t>Investments</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -945,6 +1540,125 @@
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Rent</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Transitionary</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Giving</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>LLC</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Kota</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Necessities</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -961,7 +1675,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -972,7 +1686,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Botox</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -989,7 +1703,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Income</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -1023,7 +1737,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>God</t>
+          <t>Investments</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1032,6 +1746,125 @@
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Rent</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Transitionary</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Giving</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>LLC</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Kota</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Necessities</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1048,7 +1881,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1059,7 +1892,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Botox</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -1076,7 +1909,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Income</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -1110,7 +1943,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>God</t>
+          <t>Investments</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1119,6 +1952,125 @@
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Rent</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Transitionary</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Giving</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>LLC</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Kota</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Necessities</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1135,7 +2087,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1146,7 +2098,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Botox</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -1163,7 +2115,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Income</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -1197,7 +2149,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>God</t>
+          <t>Investments</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1206,6 +2158,125 @@
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Rent</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Transitionary</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Giving</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>LLC</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Kota</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Necessities</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1222,7 +2293,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1233,7 +2304,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Botox</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -1250,7 +2321,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Income</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -1284,7 +2355,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>God</t>
+          <t>Investments</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1293,6 +2364,125 @@
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Rent</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Transitionary</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Giving</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>LLC</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Kota</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Necessities</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1309,7 +2499,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1320,7 +2510,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Botox</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -1337,7 +2527,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Income</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -1371,7 +2561,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>God</t>
+          <t>Investments</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1380,6 +2570,125 @@
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Rent</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Transitionary</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Giving</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>LLC</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Kota</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Necessities</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1396,7 +2705,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1407,7 +2716,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Botox</t>
+          <t>Gas</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -1424,7 +2733,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Gas</t>
+          <t>Income</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -1458,7 +2767,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>God</t>
+          <t>Investments</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -1467,6 +2776,125 @@
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Loan</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Rent</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Transitionary</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Giving</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>LLC</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>Kota</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Necessities</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>